<commit_message>
actualitzar mapa amb l'acreditacio de l'hospital de lleida arnau de vilanova
</commit_message>
<xml_diff>
--- a/mii/hospitals/hospitals_catalunya_geocoded.xlsx
+++ b/mii/hospitals/hospitals_catalunya_geocoded.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maciamug/Desktop/repos/regions-sanitaries-catalunya/mii/hospitals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB82B51-2C6B-374D-9145-B234A2A95354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E504F7B3-AC63-4048-B55B-16939CFAB6DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1683,8 +1683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+    <sheetView tabSelected="1" topLeftCell="F56" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="N65" sqref="N65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4743,7 +4743,7 @@
         <v>0.61337909999999995</v>
       </c>
       <c r="N65" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="O65" t="s">
         <v>414</v>

</xml_diff>